<commit_message>
Some more changes I made
</commit_message>
<xml_diff>
--- a/ButtonNumbers.xlsx
+++ b/ButtonNumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="299" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="300" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>row\col</t>
+  </si>
+  <si>
+    <t>7*row+col</t>
   </si>
 </sst>
 </file>
@@ -154,13 +157,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -350,6 +353,11 @@
         <v>41</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>